<commit_message>
update row for ipl 2025 data set
</commit_message>
<xml_diff>
--- a/TATA IPL 2025.xlsx
+++ b/TATA IPL 2025.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69916646-066A-4115-83C4-7160396BF914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{69916646-066A-4115-83C4-7160396BF914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42799D0D-84E1-416B-81BF-D7B230BB0703}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15512,7 +15512,9 @@
   </sheetPr>
   <dimension ref="A1:G229"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
@@ -16731,7 +16733,7 @@
         <v>2</v>
       </c>
       <c r="D53" s="9">
-        <v>12.25</v>
+        <v>12.29</v>
       </c>
       <c r="E53" s="8" t="s">
         <v>241</v>

</xml_diff>

<commit_message>
update noor ahmad price
</commit_message>
<xml_diff>
--- a/TATA IPL 2025.xlsx
+++ b/TATA IPL 2025.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{69916646-066A-4115-83C4-7160396BF914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42799D0D-84E1-416B-81BF-D7B230BB0703}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{69916646-066A-4115-83C4-7160396BF914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF73A90D-093F-4E1D-9FDC-17146F90DCEF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15512,8 +15512,8 @@
   </sheetPr>
   <dimension ref="A1:G229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -15652,7 +15652,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="9">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>239</v>

</xml_diff>